<commit_message>
Fixed data for all demo programs
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel33.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel33.w3mi.data.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Internal table" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Internal table'!$A$1:$G$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Internal table'!$A$1:$G$5</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>001</t>
   </si>
@@ -25,19 +25,40 @@
     <t>AD</t>
   </si>
   <si>
-    <t>AE</t>
-  </si>
-  <si>
     <t>Andorra</t>
   </si>
   <si>
+    <t>Andorran</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Belgian</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
     <t>Client</t>
   </si>
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>D</t>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
   <si>
     <t>Language</t>
@@ -46,25 +67,16 @@
     <t>Long name</t>
   </si>
   <si>
+    <t>Micronesia</t>
+  </si>
+  <si>
+    <t>Micronesian</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Nationality</t>
-  </si>
-  <si>
-    <t>Ver.Arab.Emir.</t>
-  </si>
-  <si>
-    <t>Vereinigte Arabische Emirate</t>
-  </si>
-  <si>
-    <t>andorranisch</t>
-  </si>
-  <si>
-    <t>d. Verein. Arab</t>
-  </si>
-  <si>
-    <t>v.d. Vereinigten Arabischen Emiraten</t>
   </si>
 </sst>
 </file>
@@ -418,7 +430,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" zoomScaleSheetLayoutView="100" workbookViewId="0" showGridLines="1" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,25 +449,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -463,22 +475,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" hidden="true">
@@ -486,26 +498,72 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" hidden="true">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" hidden="true">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G3">
+  <autoFilter ref="A1:G5">
     <filterColumn colId="2">
       <filters>
         <filter val="AD"/>

</xml_diff>